<commit_message>
updated commit, may 31, 2024
</commit_message>
<xml_diff>
--- a/qmd/projects/msu/wss/weather/moccasin_weather_maes.xlsx
+++ b/qmd/projects/msu/wss/weather/moccasin_weather_maes.xlsx
@@ -1,19 +1,19 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10414"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10512"/>
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://montanaedu-my.sharepoint.com/personal/n47c392_msu_montana_edu/Documents/GitHub/Quarto Website/Quarto Website/qmd/projects/msu/wss/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://montanaedu-my.sharepoint.com/personal/n47c392_msu_montana_edu/Documents/GitHub/Quarto Website/Quarto Website/qmd/projects/msu/wss/weather/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="4" documentId="8_{0317C29C-32A6-FF40-90B0-6828A60D5611}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{17D779CA-CE22-A545-8D21-A118E60C326F}"/>
+  <xr:revisionPtr revIDLastSave="5" documentId="8_{0317C29C-32A6-FF40-90B0-6828A60D5611}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{8A7857F7-C7EB-1B4E-ADF6-8821743F4A0C}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="740" windowWidth="29400" windowHeight="16880" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="prcp" sheetId="1" r:id="rId1"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -808,6 +808,10 @@
     </ext>
   </extLst>
 </styleSheet>
+</file>
+
+<file path=xl/persons/person.xml><?xml version="1.0" encoding="utf-8"?>
+<personList xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main"/>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>

</xml_diff>